<commit_message>
Fix : Song Entity 수정
- Song Entity를 수정했습니다.
</commit_message>
<xml_diff>
--- a/crawling/singer.xlsx
+++ b/crawling/singer.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4306" uniqueCount="4306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4736" uniqueCount="4736">
   <si>
     <t>6RHTUrRF63xao58xh9FXYJ</t>
   </si>
@@ -12941,6 +12941,1296 @@
   </si>
   <si>
     <t>4ylqqqUMfc5TdqwoLuq6he</t>
+  </si>
+  <si>
+    <t>6OZmjtuzO1FCcPQ6kdPF5x</t>
+  </si>
+  <si>
+    <t>5UQqgiSt6Eh19Zm58qPxPS</t>
+  </si>
+  <si>
+    <t>5HG9Eg7Ik8ZuNtMyGYTxLG</t>
+  </si>
+  <si>
+    <t>5vBh0nve44zwwVF5KWtCwA</t>
+  </si>
+  <si>
+    <t>78sEozQOEJxzXegUuqRSgH</t>
+  </si>
+  <si>
+    <t>0bouHpX4JiuPnIfP2jFxRi</t>
+  </si>
+  <si>
+    <t>0wy0KtAlsZ59mEgtmEjuUk</t>
+  </si>
+  <si>
+    <t>43wuPaPcZVMJQWLRaPR4Yz</t>
+  </si>
+  <si>
+    <t>2Habwewg0ZpMr2YWSTANE9</t>
+  </si>
+  <si>
+    <t>0mVpWDLWdc7t13qs29vnEv</t>
+  </si>
+  <si>
+    <t>2fxWL96h0S44PhEa9e6mtm</t>
+  </si>
+  <si>
+    <t>13dkPjqmbcchm8cXjEJQeP</t>
+  </si>
+  <si>
+    <t>5N1GUHhFMRFFgMTjSOJDb9</t>
+  </si>
+  <si>
+    <t>5b7OnShG0qlJM7ujj7MdnQ</t>
+  </si>
+  <si>
+    <t>7bFDJIIDPq0Gn5vI7Ce34f</t>
+  </si>
+  <si>
+    <t>5gjbJH4uF12lqYaPJfLygo</t>
+  </si>
+  <si>
+    <t>7euAAWjiEIEo1a2XkkR7wZ</t>
+  </si>
+  <si>
+    <t>6pMT9pTqG7JQlcXWj8PpSB</t>
+  </si>
+  <si>
+    <t>6f4LXqcGifD364sFBKFfoN</t>
+  </si>
+  <si>
+    <t>4iOVIMcUg6zfAPv2Dz01eq</t>
+  </si>
+  <si>
+    <t>36NfRmhEeMBlaQXAG3CP9Q</t>
+  </si>
+  <si>
+    <t>4DozkIMJBaF8L9Tix8pUID</t>
+  </si>
+  <si>
+    <t>30gSCgs3b5RPNMHVjl1RLd</t>
+  </si>
+  <si>
+    <t>5pAFKhoqlYPpCSiTOjh9Bz</t>
+  </si>
+  <si>
+    <t>1PsknnitlKhm7SOszdGWB1</t>
+  </si>
+  <si>
+    <t>00q3HI6mnGUJqMlfwBJTco</t>
+  </si>
+  <si>
+    <t>362GV7hdgLf9AHDE9l0zyn</t>
+  </si>
+  <si>
+    <t>69hDvJyXHpQoSlSZGaYoUK</t>
+  </si>
+  <si>
+    <t>3IOUX2zimWLnlS0kRyJQJq</t>
+  </si>
+  <si>
+    <t>2fFxNneQmtCTdIwEpfXnqe</t>
+  </si>
+  <si>
+    <t>7KmdcfQ5slIF0H8Smd0Tyq</t>
+  </si>
+  <si>
+    <t>3w7DwDLRBfI6SfZnLVj7AB</t>
+  </si>
+  <si>
+    <t>7d6pSr9mpmdSnxEdEjFYpF</t>
+  </si>
+  <si>
+    <t>17yd2V3A2UmwD0a00hmjX5</t>
+  </si>
+  <si>
+    <t>0bxSJJ7V2M4Zb9lpRzWPD8</t>
+  </si>
+  <si>
+    <t>4UfFGMMbPfVf1t43Za1rwo</t>
+  </si>
+  <si>
+    <t>1259XbZ4Fb9LbsGDilYf3t</t>
+  </si>
+  <si>
+    <t>2O97eRM6M6HZhPtLgMZIAk</t>
+  </si>
+  <si>
+    <t>4QLkKkxIGUpdSxtxtX79iY</t>
+  </si>
+  <si>
+    <t>5ENwCCr5vpgcwr4HgTmWGs</t>
+  </si>
+  <si>
+    <t>2xJuQfOX5eZ9hqp9nrlna8</t>
+  </si>
+  <si>
+    <t>6KKU9kDfD89Sl9mJzmoftD</t>
+  </si>
+  <si>
+    <t>0zNxCxEjUGAsb6ygZd27fC</t>
+  </si>
+  <si>
+    <t>3zbsh8As245tuzauLHqvGH</t>
+  </si>
+  <si>
+    <t>0vnjhCrXCcFwS5tw9k6DT9</t>
+  </si>
+  <si>
+    <t>76BcfRhOZ6XGgekvnFHvhr</t>
+  </si>
+  <si>
+    <t>1NggMz3y8JctYhecfAvy4l</t>
+  </si>
+  <si>
+    <t>25TosnjUS46keBElzug4NR</t>
+  </si>
+  <si>
+    <t>02lSURBnybQit6FIm8zGDE</t>
+  </si>
+  <si>
+    <t>1FMm0o9iqEKuk1B624okFn</t>
+  </si>
+  <si>
+    <t>4r1fs0uCxOqVajSaQvUQE2</t>
+  </si>
+  <si>
+    <t>6I2l37l0O5gjtj4dphiPST</t>
+  </si>
+  <si>
+    <t>0zELSN9QMUxEbhuh0hKx9l</t>
+  </si>
+  <si>
+    <t>2y3sCYh34QgmPXj1HdUlsu</t>
+  </si>
+  <si>
+    <t>7ybNybQQDnJoGOP2Y9JyHG</t>
+  </si>
+  <si>
+    <t>5yM1DQUmKUfdc4FRpgp4Cx</t>
+  </si>
+  <si>
+    <t>4TkeFolTZyiNHXse2axCOA</t>
+  </si>
+  <si>
+    <t>2crTNLaQdRWk74CNuccUOs</t>
+  </si>
+  <si>
+    <t>53sTxOQ5mNoqYdxO1heLUk</t>
+  </si>
+  <si>
+    <t>1DRKyJFDZaw42Nw3En5J1R</t>
+  </si>
+  <si>
+    <t>0erCUmNsco9OoAhaLakbsu</t>
+  </si>
+  <si>
+    <t>6lTux7kxPz3oahwoxtWxO9</t>
+  </si>
+  <si>
+    <t>6j74FeMTy0Ivy9u43YAoZn</t>
+  </si>
+  <si>
+    <t>2dWTkKrPGvkwSTSuRSwJNc</t>
+  </si>
+  <si>
+    <t>2NrfAs6msmsiqK4LPxb3sR</t>
+  </si>
+  <si>
+    <t>03hoW2fKIIlH0LwQVI2iPh</t>
+  </si>
+  <si>
+    <t>7rnHKMD15HPfqWZ09iZ4rU</t>
+  </si>
+  <si>
+    <t>6ECfS3BcHWcg6dVhkeEI3p</t>
+  </si>
+  <si>
+    <t>4e9ML6IDGbv8W09mMlStKc</t>
+  </si>
+  <si>
+    <t>2Dc5cmoiYcZNXnI6BkDHDj</t>
+  </si>
+  <si>
+    <t>16pmvDuhjGkXVcfurGFV9r</t>
+  </si>
+  <si>
+    <t>3AoHwyG0A5hOD0EywkjsSc</t>
+  </si>
+  <si>
+    <t>6E8BWapRyleJWzWxYlWuH1</t>
+  </si>
+  <si>
+    <t>6wYCHpa01ydmjizlQ6Zhrn</t>
+  </si>
+  <si>
+    <t>3dKCsLzFJuRrB3POfaMMAw</t>
+  </si>
+  <si>
+    <t>7wXonQx4XEYN8STNn9Wbuy</t>
+  </si>
+  <si>
+    <t>1cnsEyQY7zlkdK1F3BVSRm</t>
+  </si>
+  <si>
+    <t>7mLdNzBFl0GPVVXiTxiP60</t>
+  </si>
+  <si>
+    <t>1C6itWTwgfxpe9mbKDsdrv</t>
+  </si>
+  <si>
+    <t>41RdYLvKL6yRRaLAYSCf9S</t>
+  </si>
+  <si>
+    <t>6qncLwV1JU14bVepluOF2g</t>
+  </si>
+  <si>
+    <t>0mU2G4o6lh276WfSuhAClz</t>
+  </si>
+  <si>
+    <t>6EKPIs8Fi2hkJ0jtIjfcHG</t>
+  </si>
+  <si>
+    <t>0MZE7zyGdaunT5Rr56xUqD</t>
+  </si>
+  <si>
+    <t>395u0QNp2Ai3i8c4aW0oZf</t>
+  </si>
+  <si>
+    <t>44WfogQGoTuJ6Ih8LP2fFL</t>
+  </si>
+  <si>
+    <t>5lqqriVEDQinsSIYXndbcL</t>
+  </si>
+  <si>
+    <t>5DTXUiS1xN0K5ZF7oUV1SR</t>
+  </si>
+  <si>
+    <t>6bXaConafHEUo877kV9ptC</t>
+  </si>
+  <si>
+    <t>1LGJH2dqfUSE3vVyqzepg9</t>
+  </si>
+  <si>
+    <t>3988NXDQ0XzfTeYoFvkCFy</t>
+  </si>
+  <si>
+    <t>354KW4nBdSipwcu91kNwq0</t>
+  </si>
+  <si>
+    <t>5jp4JnkMXIogEOMptxnSpZ</t>
+  </si>
+  <si>
+    <t>42iv9hOHdsCtf4Um4rMEvw</t>
+  </si>
+  <si>
+    <t>0IpxVRcAYIyikzeWyasd56</t>
+  </si>
+  <si>
+    <t>2DoAIZZ9oXS2HuAvdLqICE</t>
+  </si>
+  <si>
+    <t>1StpfPAgYvblPWhlcb2Sok</t>
+  </si>
+  <si>
+    <t>3BgmYRaiq7jnjwgHdNWHSM</t>
+  </si>
+  <si>
+    <t>429OEtZSORLIdTnbeg8Pwu</t>
+  </si>
+  <si>
+    <t>0fFxDbjl7vauD7pqSlcgRh</t>
+  </si>
+  <si>
+    <t>4R9QePeIvBFcjzNujtkkiu</t>
+  </si>
+  <si>
+    <t>05z2SAl98I4vTJpz9VCAj9</t>
+  </si>
+  <si>
+    <t>2BoIxjVLj8n9buWreuvsZF</t>
+  </si>
+  <si>
+    <t>3XtsRGVgT1nUh9qVlH6Wnt</t>
+  </si>
+  <si>
+    <t>13aiEk0fFVGkLXyNMrdM7o</t>
+  </si>
+  <si>
+    <t>1WZarnZpWEv7dDtjAETt4X</t>
+  </si>
+  <si>
+    <t>3tLTzUmenYSz1FS9ijEUuX</t>
+  </si>
+  <si>
+    <t>1fneobpsKEYwpsI9inK6FP</t>
+  </si>
+  <si>
+    <t>1wy3fou4KaPxc1cp9gHqxX</t>
+  </si>
+  <si>
+    <t>0xsCXMIcnrXhRiNL11HlxP</t>
+  </si>
+  <si>
+    <t>2UBgP3zLVbeYiHs8b5aLDb</t>
+  </si>
+  <si>
+    <t>6kfcndVsu8F9Y5gL5xc717</t>
+  </si>
+  <si>
+    <t>3Th9UyipOGp08husDe0Era</t>
+  </si>
+  <si>
+    <t>0YjEWrRKD9nBJfeF5eLdBd</t>
+  </si>
+  <si>
+    <t>0neVDcSdi4GMgFduUudWve</t>
+  </si>
+  <si>
+    <t>5wDdxgQC5djHDOI6AuTnuY</t>
+  </si>
+  <si>
+    <t>4KtproRH8QOCQZLuAZ8lfw</t>
+  </si>
+  <si>
+    <t>0sbcEwgYwffJrmDZK22f9a</t>
+  </si>
+  <si>
+    <t>6bguntfj9ZnX1lFvSYl72d</t>
+  </si>
+  <si>
+    <t>4cqVlLy4QV2KwAojyE7KHR</t>
+  </si>
+  <si>
+    <t>3fy7EyjDaIZ3BNhNOv2jtQ</t>
+  </si>
+  <si>
+    <t>65IzDDRlZuKIBe0QCG68Cu</t>
+  </si>
+  <si>
+    <t>4bpY9pKx3mCQXZFO4RqsDb</t>
+  </si>
+  <si>
+    <t>5hWK63iafJeDWBEZP4ClWV</t>
+  </si>
+  <si>
+    <t>5vWbhpSiUoTcaNsleGQ5KX</t>
+  </si>
+  <si>
+    <t>1tuhmfkKlaISCMF39DicJA</t>
+  </si>
+  <si>
+    <t>47H0KicYLCLlFGNA2wwUSx</t>
+  </si>
+  <si>
+    <t>3CBAla9ztOdoq3kL7jhhIE</t>
+  </si>
+  <si>
+    <t>0RJ69PVBnwXrzH9vLQfNM5</t>
+  </si>
+  <si>
+    <t>6rh2Qeb3PJ8dFCL7F3Xuyn</t>
+  </si>
+  <si>
+    <t>6I3Ht2A9XcZyeD8cMJuIWI</t>
+  </si>
+  <si>
+    <t>2QwMi696g8ta10viltHDzF</t>
+  </si>
+  <si>
+    <t>3movVK8g1sLwRn0tG9TCbp</t>
+  </si>
+  <si>
+    <t>56c64Jn2nTwC88OugL9e6x</t>
+  </si>
+  <si>
+    <t>3sxyDfYt9DUnly19mtkg00</t>
+  </si>
+  <si>
+    <t>3ywIAyb9Meif2REfU5Gvzm</t>
+  </si>
+  <si>
+    <t>3nGcR2YPVutiP19SAuLgEM</t>
+  </si>
+  <si>
+    <t>2aCSYXdXqJNaXk99vjYnkQ</t>
+  </si>
+  <si>
+    <t>1zgpTjSOiCfzpA7KvLc3iq</t>
+  </si>
+  <si>
+    <t>5oXqe1qxOiHseFau5uRXa2</t>
+  </si>
+  <si>
+    <t>2rae1V0FMh1HkfZEPBTYko</t>
+  </si>
+  <si>
+    <t>6IRrps9hjAz3UAq2dkrjEd</t>
+  </si>
+  <si>
+    <t>5NDxEIj1zBbVtHjzwNk698</t>
+  </si>
+  <si>
+    <t>1APJsG01DVCMmU0VvCDiu5</t>
+  </si>
+  <si>
+    <t>5R47d8n2iKZiKM0C4XFKf2</t>
+  </si>
+  <si>
+    <t>73EYtYOnqjLZuejdSNtnrz</t>
+  </si>
+  <si>
+    <t>6MmYIv9BGhVlKIL0nauAQi</t>
+  </si>
+  <si>
+    <t>7z1feasBdOMH1TcKVV11Z9</t>
+  </si>
+  <si>
+    <t>7AAELF342dQSH1VSsHqwqh</t>
+  </si>
+  <si>
+    <t>24St3p1IfixsAct0pnVO0g</t>
+  </si>
+  <si>
+    <t>4sjeFC94qiXqGqnZxAvJaT</t>
+  </si>
+  <si>
+    <t>3pcy4WDjEXU6te4ZXE7l2t</t>
+  </si>
+  <si>
+    <t>79FSPaOK2holUpJ6hosFe2</t>
+  </si>
+  <si>
+    <t>2nb86NOGyE646Xgfohh4Gg</t>
+  </si>
+  <si>
+    <t>7h1HqadQlWT6nnloNiUSyC</t>
+  </si>
+  <si>
+    <t>1fkIW88TYRoOZE6VLIfSef</t>
+  </si>
+  <si>
+    <t>5l41OEmvlh9UqJgILG7ajy</t>
+  </si>
+  <si>
+    <t>0k2zyzGq6HX383VlMBOvRG</t>
+  </si>
+  <si>
+    <t>66TV1ErY4LqbhZSfhnxQ1r</t>
+  </si>
+  <si>
+    <t>3zwcvnkImdzmdgQLiYVseu</t>
+  </si>
+  <si>
+    <t>2MKcT836vEL1s5kJXJ9QNT</t>
+  </si>
+  <si>
+    <t>0w8W3eXdI5hu0GckXpu9BC</t>
+  </si>
+  <si>
+    <t>0ZUWhrUPiBZRto90P5OLMK</t>
+  </si>
+  <si>
+    <t>2aQ1wK6mP9wmumKBlvzwLP</t>
+  </si>
+  <si>
+    <t>5ye2zrfSqajyHIER3LezbP</t>
+  </si>
+  <si>
+    <t>4sCsS8JPHYMIWaIZ686UW5</t>
+  </si>
+  <si>
+    <t>4H07KDQqOFcBlz3QyYcL6j</t>
+  </si>
+  <si>
+    <t>6gTFB1mXHYHkmsCGoZIih4</t>
+  </si>
+  <si>
+    <t>0csV5zEXWTNYJA75JhSGWf</t>
+  </si>
+  <si>
+    <t>1J2RkuVj0PKrGeJV1QH9yH</t>
+  </si>
+  <si>
+    <t>28rwreOUnliu2WBefcvTPu</t>
+  </si>
+  <si>
+    <t>4pDqS4F2u1YqiR9eVXnwR9</t>
+  </si>
+  <si>
+    <t>5tXJeNZESRGJQmcLmJW4PC</t>
+  </si>
+  <si>
+    <t>6E7mVxfQQyHYogbqcbJyzX</t>
+  </si>
+  <si>
+    <t>0RNZYfVy33mwtGctVGdQ0A</t>
+  </si>
+  <si>
+    <t>4aYc6yoP53lJmEeiRj9rNt</t>
+  </si>
+  <si>
+    <t>4dKudxEVOFAAf2QzJdPZjj</t>
+  </si>
+  <si>
+    <t>1ZCJrRwwHakm5xUvVWZC9Z</t>
+  </si>
+  <si>
+    <t>0PdMNWLcoFnCZ2NXNGQHKu</t>
+  </si>
+  <si>
+    <t>6JSdWtNdhfjutA5r16UOpx</t>
+  </si>
+  <si>
+    <t>2gAmSWx7vn8ZUSFDRdte9X</t>
+  </si>
+  <si>
+    <t>1yTwwVZPzT44dkQYwitq7E</t>
+  </si>
+  <si>
+    <t>6lqx49xaWCjDrydBKnI904</t>
+  </si>
+  <si>
+    <t>0CI4rQj50Dcr30HpiD2LF6</t>
+  </si>
+  <si>
+    <t>2uLLmndNOXyB4XqMH3auYK</t>
+  </si>
+  <si>
+    <t>4f0tuIEBENmmp4JnPxV7Ka</t>
+  </si>
+  <si>
+    <t>028NwMuueNR4XG9Y3e82Tr</t>
+  </si>
+  <si>
+    <t>1SAeH1p0cDtLWrPtblmQ1s</t>
+  </si>
+  <si>
+    <t>1EkK8pp1R17bdUQ4z45TNw</t>
+  </si>
+  <si>
+    <t>1cdUc8dXboKvIZGT3sZt2R</t>
+  </si>
+  <si>
+    <t>3bLol3mD89WuxOLEvqlRmG</t>
+  </si>
+  <si>
+    <t>4k0X4tD9W1XqfGM5WT6H5l</t>
+  </si>
+  <si>
+    <t>0xxxvY5cKgFeUOf2RUzpel</t>
+  </si>
+  <si>
+    <t>5ScyNOzCMYCqYAJHPjO1ci</t>
+  </si>
+  <si>
+    <t>55I3tU4bmJi7j3RVMY0sMp</t>
+  </si>
+  <si>
+    <t>7aqMwq8bjZWoaNw3j6tOLl</t>
+  </si>
+  <si>
+    <t>7xfrM8H5HoOFQHIwGN5EbB</t>
+  </si>
+  <si>
+    <t>1T44kWQsaCh6VLltor1DFk</t>
+  </si>
+  <si>
+    <t>1d7pFQav11WQv3cXnNAWck</t>
+  </si>
+  <si>
+    <t>0pm0LWiklLtNXUP2GVwdqY</t>
+  </si>
+  <si>
+    <t>0rmB1nZVDjwoCN3kQVS7UZ</t>
+  </si>
+  <si>
+    <t>3KtQFp8FUbQMx3bLNKCw3R</t>
+  </si>
+  <si>
+    <t>6ncNdxBc8zVWMOF7nJ5Pgy</t>
+  </si>
+  <si>
+    <t>14xcm4N4Wb4BzbS5gwR4IA</t>
+  </si>
+  <si>
+    <t>60myKJRhCUEUllMdqOCzHM</t>
+  </si>
+  <si>
+    <t>4x4r99t13eG9YSKLlhdB9r</t>
+  </si>
+  <si>
+    <t>5Ac7rBwAF2MX98ku1isuhy</t>
+  </si>
+  <si>
+    <t>1wpa0c7nHGleRcXS74t1WZ</t>
+  </si>
+  <si>
+    <t>27VUbxA9iZuCNRwNRVohoP</t>
+  </si>
+  <si>
+    <t>2lSkKXr7byxMiwMvrPQBGE</t>
+  </si>
+  <si>
+    <t>4aGnfZCmSvUEDuaJ6fMlrE</t>
+  </si>
+  <si>
+    <t>28Bn2PxtmXD8UbBSM968Fp</t>
+  </si>
+  <si>
+    <t>0ufn7M4jawS5MQ03CIluFo</t>
+  </si>
+  <si>
+    <t>6ELpC1O8p5SD9oiNvJurt5</t>
+  </si>
+  <si>
+    <t>0oaOc1sdr4AeSzqL8w5ndo</t>
+  </si>
+  <si>
+    <t>0ZxH5Q8ruEBzDq5DuF6X2K</t>
+  </si>
+  <si>
+    <t>3uAZQWPMvD19hIhFI6TWgN</t>
+  </si>
+  <si>
+    <t>5Kb0Qf13EyYtVJvzCdI9M7</t>
+  </si>
+  <si>
+    <t>1dk8ZJIE1IET4n4LrxzD6I</t>
+  </si>
+  <si>
+    <t>3xYzk2kbx3IEGo2YPeoggv</t>
+  </si>
+  <si>
+    <t>1mlJpazSMM0qkokoS6SNRN</t>
+  </si>
+  <si>
+    <t>2DSGVqA0JXE2L2JqVPTuF7</t>
+  </si>
+  <si>
+    <t>5vJAuQf7YI4bRYev7UfZDs</t>
+  </si>
+  <si>
+    <t>3i67VvAwUlOKZa3fc75zs8</t>
+  </si>
+  <si>
+    <t>36qooOkbokPscdOGWHPFk7</t>
+  </si>
+  <si>
+    <t>7bdwlNOPsycFColkPRlNxY</t>
+  </si>
+  <si>
+    <t>6mWZj1Lhb9V1ZbYL5UaZ4v</t>
+  </si>
+  <si>
+    <t>4GN4kZWO3WUJz4vNM179pU</t>
+  </si>
+  <si>
+    <t>1IkWWt9qbVHIG0esJFOGqf</t>
+  </si>
+  <si>
+    <t>0gOrXuu1vCBXe3pwTyb5Ca</t>
+  </si>
+  <si>
+    <t>0yPINB4V6U9g9i9iLRRJjx</t>
+  </si>
+  <si>
+    <t>4Tn9hDjPZPTloCTtLcHkDl</t>
+  </si>
+  <si>
+    <t>1q5u8LnvomvAmiMhg8kRDp</t>
+  </si>
+  <si>
+    <t>1VTv19vFoeiKs28gOzntpL</t>
+  </si>
+  <si>
+    <t>6lA59rirEDW0rZFUV0TfCu</t>
+  </si>
+  <si>
+    <t>5VwpzhkGxagJjxn4jeK1RU</t>
+  </si>
+  <si>
+    <t>4PiqWnfbWGcCFT2UDxKCf1</t>
+  </si>
+  <si>
+    <t>4gBAA2nKYYBUsr01k0EVY4</t>
+  </si>
+  <si>
+    <t>7501C4PyvqS1BWbmrYq3LF</t>
+  </si>
+  <si>
+    <t>3xSs5iXfAy7FPN8cUqBEfm</t>
+  </si>
+  <si>
+    <t>1YoSYNmMHPZEa2WNNUS1oP</t>
+  </si>
+  <si>
+    <t>0KZ83Y1bF24W54rmvP2qxr</t>
+  </si>
+  <si>
+    <t>2eIwiMzHBYVTZ2iTYiuacE</t>
+  </si>
+  <si>
+    <t>2imvddeWiv58tUPKh8q3kO</t>
+  </si>
+  <si>
+    <t>6fs2or0cKLEM2xohWq8SoX</t>
+  </si>
+  <si>
+    <t>1SLtuLzX7bWXs78mRvEsM1</t>
+  </si>
+  <si>
+    <t>6Gq0C9ThUhlwolmce3vdok</t>
+  </si>
+  <si>
+    <t>1hliskWXXblmLcokaMUjhY</t>
+  </si>
+  <si>
+    <t>3H5gxDxZMNEJWIzO8a8yMh</t>
+  </si>
+  <si>
+    <t>0bsPYp1WhWsRaL4UD7UuYy</t>
+  </si>
+  <si>
+    <t>1KZYhJ6IFUF2oXHP5PsBhY</t>
+  </si>
+  <si>
+    <t>7BiuDGcNbiXpbmjd0F8pWc</t>
+  </si>
+  <si>
+    <t>5DRMI6KlmzFyY5ORIhdt8w</t>
+  </si>
+  <si>
+    <t>5vejKtSh2J9QVzVOzvGzOz</t>
+  </si>
+  <si>
+    <t>6UIkUxi26u7HTH8ov8AXyM</t>
+  </si>
+  <si>
+    <t>7MlrqShwBuHbkK2UsFIzuW</t>
+  </si>
+  <si>
+    <t>1LnnQiUfT4zTrL9AYYgTHq</t>
+  </si>
+  <si>
+    <t>0COk0aZRtuQ2oWwE8oNis7</t>
+  </si>
+  <si>
+    <t>43LrKq9HELjNj0p44d4uOj</t>
+  </si>
+  <si>
+    <t>61kLMGHK5jlUC1chnHBPlc</t>
+  </si>
+  <si>
+    <t>1H372XKZbJKCH3zAhnuQYD</t>
+  </si>
+  <si>
+    <t>5loGOjocD25ID7iaUx5K28</t>
+  </si>
+  <si>
+    <t>4o1yQsUjRLHqaZqPlpuSVs</t>
+  </si>
+  <si>
+    <t>33m7gT6eP9unPArdo8wfbr</t>
+  </si>
+  <si>
+    <t>0LLuMNGk0hEVjPuEBNaNO1</t>
+  </si>
+  <si>
+    <t>2MehGNUhZweLVKrxjDpfVa</t>
+  </si>
+  <si>
+    <t>2Lg7vSM7bduFnSr4nM9OdA</t>
+  </si>
+  <si>
+    <t>6T6voh1NTMXcpa2aNlXMko</t>
+  </si>
+  <si>
+    <t>1kihDFapa9lm74coxVObtL</t>
+  </si>
+  <si>
+    <t>1bR457yJADpHOckKNHdPM6</t>
+  </si>
+  <si>
+    <t>5jUOJXu5KfSn7ZXlPveyuQ</t>
+  </si>
+  <si>
+    <t>0p7iv1Q28yJwB6pMFphIv9</t>
+  </si>
+  <si>
+    <t>3a3LDEkR20md8TlZk0zTrL</t>
+  </si>
+  <si>
+    <t>71DxJPh5DvBfI8MjQI7qDE</t>
+  </si>
+  <si>
+    <t>1rVpXgPDVeUXPKKqVEnAGb</t>
+  </si>
+  <si>
+    <t>4XkyKEhzoNQEg8ruN7OkPs</t>
+  </si>
+  <si>
+    <t>3Gka2tZrE8vX4fBFtgknqB</t>
+  </si>
+  <si>
+    <t>5X5g8sGWyeNuiqsg8sfMzH</t>
+  </si>
+  <si>
+    <t>27T030eWyCQRmDyuvr1kxY</t>
+  </si>
+  <si>
+    <t>4vofk7SmQmc997Tkoic0O5</t>
+  </si>
+  <si>
+    <t>3JysSUOyfVs1UQ0UaESheP</t>
+  </si>
+  <si>
+    <t>1IQ2e1buppatiN1bxUVkrk</t>
+  </si>
+  <si>
+    <t>0DCw6lHkzh9t7f8Hb4Z0Sx</t>
+  </si>
+  <si>
+    <t>0TILJJ3OI8J9tJ50NE33Kl</t>
+  </si>
+  <si>
+    <t>4W3AJWKiTqHppKh6ameRrK</t>
+  </si>
+  <si>
+    <t>57ylwQTnFnIhJh4nu4rxCs</t>
+  </si>
+  <si>
+    <t>28hJdGN1Awf7u3ifk2lVkg</t>
+  </si>
+  <si>
+    <t>4PBdWAjtlDwQgWfGjsjQtD</t>
+  </si>
+  <si>
+    <t>64tNsm6TnZe2zpcMVMOoHL</t>
+  </si>
+  <si>
+    <t>2ZeeJPDvqzQ7c8iG3rRsyc</t>
+  </si>
+  <si>
+    <t>0iGR1dPENdfzoZbpsFlYug</t>
+  </si>
+  <si>
+    <t>5FGnjqVQ2v6N5BLsBwYwPP</t>
+  </si>
+  <si>
+    <t>6KyAMbfO1f5yIQjh9WWYDa</t>
+  </si>
+  <si>
+    <t>3uaX4vj7m3bkWhcY9xooJ6</t>
+  </si>
+  <si>
+    <t>25OMfKk5AnZxUdzwDy3bOj</t>
+  </si>
+  <si>
+    <t>40X7tXw4Tk4m5WFDfGJnZe</t>
+  </si>
+  <si>
+    <t>1zqdtfOwTbQRPqj7wTEHa5</t>
+  </si>
+  <si>
+    <t>3BF7sUICDYsxrGIanZQ3o5</t>
+  </si>
+  <si>
+    <t>4Jk4X8SThiE5yK5mpvLtba</t>
+  </si>
+  <si>
+    <t>1aQyW9SLtSSpPHbjYAy35F</t>
+  </si>
+  <si>
+    <t>5yES1lbfHCYiyoMu2lytl3</t>
+  </si>
+  <si>
+    <t>3tAbMWoqqMd4XywxVIrVwU</t>
+  </si>
+  <si>
+    <t>5Gr2GZcljB4TQEULKoYb0q</t>
+  </si>
+  <si>
+    <t>4uaGojdWj4H6cTJydZUPWG</t>
+  </si>
+  <si>
+    <t>5Mk3yOBlfweeKamsDiap8H</t>
+  </si>
+  <si>
+    <t>3vcmFdngDnToTjWO61hMTK</t>
+  </si>
+  <si>
+    <t>6LszZyd03prLB8lIPbZ9Uo</t>
+  </si>
+  <si>
+    <t>4kwRGpvKw9YsV0DTRZQKyH</t>
+  </si>
+  <si>
+    <t>09O5HSw8RO3aAnWNCADaKS</t>
+  </si>
+  <si>
+    <t>5zLd9DhI6ebR8fvwunp4bX</t>
+  </si>
+  <si>
+    <t>33crDRqANd3NQHJagZkQ7O</t>
+  </si>
+  <si>
+    <t>1vSjt7d3bXlGe8pQsDOjyl</t>
+  </si>
+  <si>
+    <t>1cycjRW4LjxhpdSy9Z6Iw2</t>
+  </si>
+  <si>
+    <t>0D3okj3uWTBA0Lf61dqu4F</t>
+  </si>
+  <si>
+    <t>2jW6U2KrLUXb3HmKyaMRfS</t>
+  </si>
+  <si>
+    <t>1fXuDbMW1OiHYxwlzyI32S</t>
+  </si>
+  <si>
+    <t>1r4Kg6QvOag5akux2LZIDx</t>
+  </si>
+  <si>
+    <t>2jLk7mJoU5eqrZBTi8E22c</t>
+  </si>
+  <si>
+    <t>6gU2BZ54QXB1bAYNqCLUc3</t>
+  </si>
+  <si>
+    <t>4Rd6lGWGMdbVJHH6fsv3vO</t>
+  </si>
+  <si>
+    <t>0BtDdJ64d2YtiHFNoFvpdn</t>
+  </si>
+  <si>
+    <t>0dmr6iGzWoe0oDsCGOjAa9</t>
+  </si>
+  <si>
+    <t>0bLzal7T67B0KZBfgQDM7I</t>
+  </si>
+  <si>
+    <t>3J9r5Bq4ZddNLatsd0bJWb</t>
+  </si>
+  <si>
+    <t>5674o7JD1sMbgpoQUiWOIc</t>
+  </si>
+  <si>
+    <t>2YSSfMg2K75oTvfc63kGQB</t>
+  </si>
+  <si>
+    <t>0Z9ba766fVlqIYuA2jm0e4</t>
+  </si>
+  <si>
+    <t>1a1SeoN2d5eEvRlkJJ9TIo</t>
+  </si>
+  <si>
+    <t>6yxXsPXcgTJjBRelX9NCiF</t>
+  </si>
+  <si>
+    <t>0sSAFVekiDtX7PXDQvHnlK</t>
+  </si>
+  <si>
+    <t>7zn5DkieqX8VqOeDi1sHoz</t>
+  </si>
+  <si>
+    <t>1htPJUlogkZBjbKp86uuLF</t>
+  </si>
+  <si>
+    <t>54JXhmpGDN8NdAIq44z4gt</t>
+  </si>
+  <si>
+    <t>6aQjwZOj9cjAtErrzI03RR</t>
+  </si>
+  <si>
+    <t>0L4d5EwDWqTEOTjztWF0mw</t>
+  </si>
+  <si>
+    <t>27PLs0B6sCcweXaiFhAdwH</t>
+  </si>
+  <si>
+    <t>38dAQZvNchr4zg7Sg01KIn</t>
+  </si>
+  <si>
+    <t>2PAdY3cUwkya3iXBv0GSm0</t>
+  </si>
+  <si>
+    <t>1R5iQMzT9jP5DIzVGPmWy6</t>
+  </si>
+  <si>
+    <t>3xwV7Ve41xbvOk2BVCHqEf</t>
+  </si>
+  <si>
+    <t>5rGTIicetUCmoXHgpU7fKz</t>
+  </si>
+  <si>
+    <t>0Q4wv11yD3N6MhSxCjfSet</t>
+  </si>
+  <si>
+    <t>1R4kc8WcmmFEn7lFvPeJ5E</t>
+  </si>
+  <si>
+    <t>4a8F4QBYAiskVyQjk9mlpl</t>
+  </si>
+  <si>
+    <t>5NOUPpTUG8w2NRrYGSUsIf</t>
+  </si>
+  <si>
+    <t>6eY9LT0jokuZ4iwGoAW9nt</t>
+  </si>
+  <si>
+    <t>6vIhDRhF3mx8BFNPMvFAiF</t>
+  </si>
+  <si>
+    <t>6XGZjwivb9dZlSxfiv0pYU</t>
+  </si>
+  <si>
+    <t>1V618lgufRCeR9ilSwZB7h</t>
+  </si>
+  <si>
+    <t>2DPb4rebme0svdWDLPz4dc</t>
+  </si>
+  <si>
+    <t>79woHgucZjWY8K6nIkCEMI</t>
+  </si>
+  <si>
+    <t>0j8Oj83l1lzfPlaA7qQM0u</t>
+  </si>
+  <si>
+    <t>7vCxULrsp3UyRkvHiB3Of6</t>
+  </si>
+  <si>
+    <t>07Qt0KlMf6vpPVXuY5Qrhj</t>
+  </si>
+  <si>
+    <t>4zzzvh8xX7laDArf8Gt7iw</t>
+  </si>
+  <si>
+    <t>420WywYXnWiFsRAqeIuMZq</t>
+  </si>
+  <si>
+    <t>6os3vXz4NNdQ0Vz3Ht0vpO</t>
+  </si>
+  <si>
+    <t>4HyzwDBcs7BsvF2ggeCny6</t>
+  </si>
+  <si>
+    <t>3HlM1dEHdhaFFtKxAZ3M15</t>
+  </si>
+  <si>
+    <t>7gZVmlobk0KC6ZfxOD52hH</t>
+  </si>
+  <si>
+    <t>62oYdsAy450XtCfdIrV9Bl</t>
+  </si>
+  <si>
+    <t>3RyP9efTESjn78QR2NMjra</t>
+  </si>
+  <si>
+    <t>48l7QsNEqTci1mvm7gMuoe</t>
+  </si>
+  <si>
+    <t>0tObvGdIPuiOvMOxcRajKn</t>
+  </si>
+  <si>
+    <t>281f9Xcai3LC2cQxF4A4ux</t>
+  </si>
+  <si>
+    <t>2wTWfen940n9t7jrsvaHQV</t>
+  </si>
+  <si>
+    <t>5yDDlf63Na65co2arRdYn0</t>
+  </si>
+  <si>
+    <t>6yC7v5MUs8vO5VyHhqr6V1</t>
+  </si>
+  <si>
+    <t>6OewwhXIpzSzlsiG9X6LOX</t>
+  </si>
+  <si>
+    <t>1cMn5ZdQibv1JyQdmuxeHB</t>
+  </si>
+  <si>
+    <t>0qNxI0JfVLTxRNKE5LYdAu</t>
+  </si>
+  <si>
+    <t>0xh7fPy14EdEhtf003KzTg</t>
+  </si>
+  <si>
+    <t>6sA3g4kSpQnDHd5o5gssrE</t>
+  </si>
+  <si>
+    <t>1MturlEnPcoybcsZbrdEPB</t>
+  </si>
+  <si>
+    <t>7Jl4Y7b1Wi2vQLkCiwaVED</t>
+  </si>
+  <si>
+    <t>2BzEJybfRAL6DxCeYW2e7G</t>
+  </si>
+  <si>
+    <t>414TGZEIhgEl3bJv13BAsG</t>
+  </si>
+  <si>
+    <t>5qGm12nyHOXgOpAsHQWwtV</t>
+  </si>
+  <si>
+    <t>2MOlaeCGL8W2BKETEpiQhc</t>
+  </si>
+  <si>
+    <t>16UoIs2XQBPrSg0LAH0N9y</t>
+  </si>
+  <si>
+    <t>0bODDKcuCOiFlp6UhiojO7</t>
+  </si>
+  <si>
+    <t>02CZbwDYyHWBQeWabWY4RM</t>
+  </si>
+  <si>
+    <t>6wDE43fDrn0khXMlj5jJHJ</t>
+  </si>
+  <si>
+    <t>4KJNczzAoOBUeW3K0WUpph</t>
+  </si>
+  <si>
+    <t>7MCd8V8S3fJVtKa1NZGk3N</t>
+  </si>
+  <si>
+    <t>18jYBTlhX9Rq8zv60jpToD</t>
+  </si>
+  <si>
+    <t>1aojb4lyc8tDVKQwFz5o4C</t>
+  </si>
+  <si>
+    <t>39kw25A0Vbx58mGBhzPZXz</t>
+  </si>
+  <si>
+    <t>7w0qj2HiAPIeUcoPogvOZ6</t>
+  </si>
+  <si>
+    <t>6nj8vLX0iYmWmx3itkEnrI</t>
+  </si>
+  <si>
+    <t>0630rYsw1mCdNfl8E3qqm2</t>
+  </si>
+  <si>
+    <t>1YhVEBLYkYdYsPw8Gh7BnI</t>
+  </si>
+  <si>
+    <t>7GH65UbP1uRY9HtNvq4R9Y</t>
+  </si>
+  <si>
+    <t>4Zop0zkYmho9A58QPgVlDK</t>
+  </si>
+  <si>
+    <t>4D1JoQ2bhE1vA7EmnnYC0E</t>
+  </si>
+  <si>
+    <t>6py9Tt8bSLtTe4vTx3iQ1O</t>
+  </si>
+  <si>
+    <t>4R6895dmKO8t5Y9mWji99d</t>
+  </si>
+  <si>
+    <t>03SZ5zVrrY9ydcNEqpaQrZ</t>
+  </si>
+  <si>
+    <t>6anJ9yWyrJuZ21vZATPnXI</t>
+  </si>
+  <si>
+    <t>4szVIYS0W4GAtsNY2mUQOp</t>
+  </si>
+  <si>
+    <t>4z6dlDfmoZstfKLVC60nM0</t>
+  </si>
+  <si>
+    <t>3RUGMx9yxNg3lltGmkTB2I</t>
+  </si>
+  <si>
+    <t>2dWFggqo9Ob31YW0SAIeuO</t>
+  </si>
+  <si>
+    <t>63jASK5GkDHb5f9zCsOyem</t>
+  </si>
+  <si>
+    <t>6cZwAByKmb7tZhpHTLdU8b</t>
+  </si>
+  <si>
+    <t>5fmLyWgIfAkbsFjMnwoWu7</t>
+  </si>
+  <si>
+    <t>5HZ0WzJwZa38S1adyyeVrY</t>
+  </si>
+  <si>
+    <t>73uO0irhYkEsOdWjBmAl3f</t>
+  </si>
+  <si>
+    <t>1sWPJ06Ed62WqGtrPUY4fa</t>
+  </si>
+  <si>
+    <t>2SFBZgfO2H1nVSgjxzJLUy</t>
+  </si>
+  <si>
+    <t>23g65hwLAhIc38UPUsqNtc</t>
+  </si>
+  <si>
+    <t>4XoFqKtEQHiuxL8CmVXLOO</t>
+  </si>
+  <si>
+    <t>3SK3gLBgy1jRuA4VnLlcs8</t>
+  </si>
+  <si>
+    <t>2RWHmppBK4tjdqxtuesmZI</t>
+  </si>
+  <si>
+    <t>5moBlpk9BYtujdRW6VLepL</t>
+  </si>
+  <si>
+    <t>4pFlv4QVInj7bAo0MqHpwW</t>
+  </si>
+  <si>
+    <t>0zdBW3w3XzBuPMUEiarUUw</t>
+  </si>
+  <si>
+    <t>3PvnWE1kf8UcjQnlFUhD5B</t>
+  </si>
+  <si>
+    <t>74qCFeNvjcO4R0cRXik17C</t>
+  </si>
+  <si>
+    <t>2OHnFY58Dg8c2SC2PtootB</t>
+  </si>
+  <si>
+    <t>6myXAUJ8cAp5oSXId946SJ</t>
+  </si>
+  <si>
+    <t>3BbwO46TU61EPYFcC9l9Lq</t>
+  </si>
+  <si>
+    <t>13Tfk6ZpGdF0G3v9B3kasP</t>
+  </si>
+  <si>
+    <t>6uELdghdD8aUe94aDyyMCK</t>
+  </si>
+  <si>
+    <t>5dz9lXIYillOvg5xH0t5EN</t>
+  </si>
+  <si>
+    <t>5pLMWE1tVs9C7F9Qqauo44</t>
+  </si>
+  <si>
+    <t>1pfkP92biveJzJLW5JGm8Z</t>
+  </si>
+  <si>
+    <t>3fcsflK8xu26XH4OYTcm5T</t>
+  </si>
+  <si>
+    <t>2LnE7uKchgVW2Uv7vzwixZ</t>
+  </si>
+  <si>
+    <t>6ILd69yy67k6OU7cwpGNSl</t>
   </si>
 </sst>
 </file>
@@ -13300,7 +14590,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G4306"/>
+  <dimension ref="A1:G4736"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2900" workbookViewId="0">
       <selection activeCell="H2837" sqref="H2837"/>
@@ -36157,6 +37447,2156 @@
         <v>4305</v>
       </c>
     </row>
+    <row r="4307">
+      <c r="A4307" t="s" s="4">
+        <v>4306</v>
+      </c>
+    </row>
+    <row r="4308">
+      <c r="A4308" t="s" s="4">
+        <v>4307</v>
+      </c>
+    </row>
+    <row r="4309">
+      <c r="A4309" t="s" s="4">
+        <v>4308</v>
+      </c>
+    </row>
+    <row r="4310">
+      <c r="A4310" t="s" s="4">
+        <v>4309</v>
+      </c>
+    </row>
+    <row r="4311">
+      <c r="A4311" t="s" s="4">
+        <v>4310</v>
+      </c>
+    </row>
+    <row r="4312">
+      <c r="A4312" t="s" s="4">
+        <v>4311</v>
+      </c>
+    </row>
+    <row r="4313">
+      <c r="A4313" t="s" s="4">
+        <v>4312</v>
+      </c>
+    </row>
+    <row r="4314">
+      <c r="A4314" t="s" s="4">
+        <v>4313</v>
+      </c>
+    </row>
+    <row r="4315">
+      <c r="A4315" t="s" s="4">
+        <v>4314</v>
+      </c>
+    </row>
+    <row r="4316">
+      <c r="A4316" t="s" s="4">
+        <v>4315</v>
+      </c>
+    </row>
+    <row r="4317">
+      <c r="A4317" t="s" s="4">
+        <v>4316</v>
+      </c>
+    </row>
+    <row r="4318">
+      <c r="A4318" t="s" s="4">
+        <v>4317</v>
+      </c>
+    </row>
+    <row r="4319">
+      <c r="A4319" t="s" s="4">
+        <v>4318</v>
+      </c>
+    </row>
+    <row r="4320">
+      <c r="A4320" t="s" s="4">
+        <v>4319</v>
+      </c>
+    </row>
+    <row r="4321">
+      <c r="A4321" t="s" s="4">
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="4322">
+      <c r="A4322" t="s" s="4">
+        <v>4321</v>
+      </c>
+    </row>
+    <row r="4323">
+      <c r="A4323" t="s" s="4">
+        <v>4322</v>
+      </c>
+    </row>
+    <row r="4324">
+      <c r="A4324" t="s" s="4">
+        <v>4323</v>
+      </c>
+    </row>
+    <row r="4325">
+      <c r="A4325" t="s" s="4">
+        <v>4324</v>
+      </c>
+    </row>
+    <row r="4326">
+      <c r="A4326" t="s" s="4">
+        <v>4325</v>
+      </c>
+    </row>
+    <row r="4327">
+      <c r="A4327" t="s" s="4">
+        <v>4326</v>
+      </c>
+    </row>
+    <row r="4328">
+      <c r="A4328" t="s" s="4">
+        <v>4327</v>
+      </c>
+    </row>
+    <row r="4329">
+      <c r="A4329" t="s" s="4">
+        <v>4328</v>
+      </c>
+    </row>
+    <row r="4330">
+      <c r="A4330" t="s" s="4">
+        <v>4329</v>
+      </c>
+    </row>
+    <row r="4331">
+      <c r="A4331" t="s" s="4">
+        <v>4330</v>
+      </c>
+    </row>
+    <row r="4332">
+      <c r="A4332" t="s" s="4">
+        <v>4331</v>
+      </c>
+    </row>
+    <row r="4333">
+      <c r="A4333" t="s" s="4">
+        <v>4332</v>
+      </c>
+    </row>
+    <row r="4334">
+      <c r="A4334" t="s" s="4">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="4335">
+      <c r="A4335" t="s" s="4">
+        <v>4334</v>
+      </c>
+    </row>
+    <row r="4336">
+      <c r="A4336" t="s" s="4">
+        <v>4335</v>
+      </c>
+    </row>
+    <row r="4337">
+      <c r="A4337" t="s" s="4">
+        <v>4336</v>
+      </c>
+    </row>
+    <row r="4338">
+      <c r="A4338" t="s" s="4">
+        <v>4337</v>
+      </c>
+    </row>
+    <row r="4339">
+      <c r="A4339" t="s" s="4">
+        <v>4338</v>
+      </c>
+    </row>
+    <row r="4340">
+      <c r="A4340" t="s" s="4">
+        <v>4339</v>
+      </c>
+    </row>
+    <row r="4341">
+      <c r="A4341" t="s" s="4">
+        <v>4340</v>
+      </c>
+    </row>
+    <row r="4342">
+      <c r="A4342" t="s" s="4">
+        <v>4341</v>
+      </c>
+    </row>
+    <row r="4343">
+      <c r="A4343" t="s" s="4">
+        <v>4342</v>
+      </c>
+    </row>
+    <row r="4344">
+      <c r="A4344" t="s" s="4">
+        <v>4343</v>
+      </c>
+    </row>
+    <row r="4345">
+      <c r="A4345" t="s" s="4">
+        <v>4344</v>
+      </c>
+    </row>
+    <row r="4346">
+      <c r="A4346" t="s" s="4">
+        <v>4345</v>
+      </c>
+    </row>
+    <row r="4347">
+      <c r="A4347" t="s" s="4">
+        <v>4346</v>
+      </c>
+    </row>
+    <row r="4348">
+      <c r="A4348" t="s" s="4">
+        <v>4347</v>
+      </c>
+    </row>
+    <row r="4349">
+      <c r="A4349" t="s" s="4">
+        <v>4348</v>
+      </c>
+    </row>
+    <row r="4350">
+      <c r="A4350" t="s" s="4">
+        <v>4349</v>
+      </c>
+    </row>
+    <row r="4351">
+      <c r="A4351" t="s" s="4">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="4352">
+      <c r="A4352" t="s" s="4">
+        <v>4351</v>
+      </c>
+    </row>
+    <row r="4353">
+      <c r="A4353" t="s" s="4">
+        <v>4352</v>
+      </c>
+    </row>
+    <row r="4354">
+      <c r="A4354" t="s" s="4">
+        <v>4353</v>
+      </c>
+    </row>
+    <row r="4355">
+      <c r="A4355" t="s" s="4">
+        <v>4354</v>
+      </c>
+    </row>
+    <row r="4356">
+      <c r="A4356" t="s" s="4">
+        <v>4355</v>
+      </c>
+    </row>
+    <row r="4357">
+      <c r="A4357" t="s" s="4">
+        <v>4356</v>
+      </c>
+    </row>
+    <row r="4358">
+      <c r="A4358" t="s" s="4">
+        <v>4357</v>
+      </c>
+    </row>
+    <row r="4359">
+      <c r="A4359" t="s" s="4">
+        <v>4358</v>
+      </c>
+    </row>
+    <row r="4360">
+      <c r="A4360" t="s" s="4">
+        <v>4359</v>
+      </c>
+    </row>
+    <row r="4361">
+      <c r="A4361" t="s" s="4">
+        <v>4360</v>
+      </c>
+    </row>
+    <row r="4362">
+      <c r="A4362" t="s" s="4">
+        <v>4361</v>
+      </c>
+    </row>
+    <row r="4363">
+      <c r="A4363" t="s" s="4">
+        <v>4362</v>
+      </c>
+    </row>
+    <row r="4364">
+      <c r="A4364" t="s" s="4">
+        <v>4363</v>
+      </c>
+    </row>
+    <row r="4365">
+      <c r="A4365" t="s" s="4">
+        <v>4364</v>
+      </c>
+    </row>
+    <row r="4366">
+      <c r="A4366" t="s" s="4">
+        <v>4365</v>
+      </c>
+    </row>
+    <row r="4367">
+      <c r="A4367" t="s" s="4">
+        <v>4366</v>
+      </c>
+    </row>
+    <row r="4368">
+      <c r="A4368" t="s" s="4">
+        <v>4367</v>
+      </c>
+    </row>
+    <row r="4369">
+      <c r="A4369" t="s" s="4">
+        <v>4368</v>
+      </c>
+    </row>
+    <row r="4370">
+      <c r="A4370" t="s" s="4">
+        <v>4369</v>
+      </c>
+    </row>
+    <row r="4371">
+      <c r="A4371" t="s" s="4">
+        <v>4370</v>
+      </c>
+    </row>
+    <row r="4372">
+      <c r="A4372" t="s" s="4">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="4373">
+      <c r="A4373" t="s" s="4">
+        <v>4372</v>
+      </c>
+    </row>
+    <row r="4374">
+      <c r="A4374" t="s" s="4">
+        <v>4373</v>
+      </c>
+    </row>
+    <row r="4375">
+      <c r="A4375" t="s" s="4">
+        <v>4374</v>
+      </c>
+    </row>
+    <row r="4376">
+      <c r="A4376" t="s" s="4">
+        <v>4375</v>
+      </c>
+    </row>
+    <row r="4377">
+      <c r="A4377" t="s" s="4">
+        <v>4376</v>
+      </c>
+    </row>
+    <row r="4378">
+      <c r="A4378" t="s" s="4">
+        <v>4377</v>
+      </c>
+    </row>
+    <row r="4379">
+      <c r="A4379" t="s" s="4">
+        <v>4378</v>
+      </c>
+    </row>
+    <row r="4380">
+      <c r="A4380" t="s" s="4">
+        <v>4379</v>
+      </c>
+    </row>
+    <row r="4381">
+      <c r="A4381" t="s" s="4">
+        <v>4380</v>
+      </c>
+    </row>
+    <row r="4382">
+      <c r="A4382" t="s" s="4">
+        <v>4381</v>
+      </c>
+    </row>
+    <row r="4383">
+      <c r="A4383" t="s" s="4">
+        <v>4382</v>
+      </c>
+    </row>
+    <row r="4384">
+      <c r="A4384" t="s" s="4">
+        <v>4383</v>
+      </c>
+    </row>
+    <row r="4385">
+      <c r="A4385" t="s" s="4">
+        <v>4384</v>
+      </c>
+    </row>
+    <row r="4386">
+      <c r="A4386" t="s" s="4">
+        <v>4385</v>
+      </c>
+    </row>
+    <row r="4387">
+      <c r="A4387" t="s" s="4">
+        <v>4386</v>
+      </c>
+    </row>
+    <row r="4388">
+      <c r="A4388" t="s" s="4">
+        <v>4387</v>
+      </c>
+    </row>
+    <row r="4389">
+      <c r="A4389" t="s" s="4">
+        <v>4388</v>
+      </c>
+    </row>
+    <row r="4390">
+      <c r="A4390" t="s" s="4">
+        <v>4389</v>
+      </c>
+    </row>
+    <row r="4391">
+      <c r="A4391" t="s" s="4">
+        <v>4390</v>
+      </c>
+    </row>
+    <row r="4392">
+      <c r="A4392" t="s" s="4">
+        <v>4391</v>
+      </c>
+    </row>
+    <row r="4393">
+      <c r="A4393" t="s" s="4">
+        <v>4392</v>
+      </c>
+    </row>
+    <row r="4394">
+      <c r="A4394" t="s" s="4">
+        <v>4393</v>
+      </c>
+    </row>
+    <row r="4395">
+      <c r="A4395" t="s" s="4">
+        <v>4394</v>
+      </c>
+    </row>
+    <row r="4396">
+      <c r="A4396" t="s" s="4">
+        <v>4395</v>
+      </c>
+    </row>
+    <row r="4397">
+      <c r="A4397" t="s" s="4">
+        <v>4396</v>
+      </c>
+    </row>
+    <row r="4398">
+      <c r="A4398" t="s" s="4">
+        <v>4397</v>
+      </c>
+    </row>
+    <row r="4399">
+      <c r="A4399" t="s" s="4">
+        <v>4398</v>
+      </c>
+    </row>
+    <row r="4400">
+      <c r="A4400" t="s" s="4">
+        <v>4399</v>
+      </c>
+    </row>
+    <row r="4401">
+      <c r="A4401" t="s" s="4">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="4402">
+      <c r="A4402" t="s" s="4">
+        <v>4401</v>
+      </c>
+    </row>
+    <row r="4403">
+      <c r="A4403" t="s" s="4">
+        <v>4402</v>
+      </c>
+    </row>
+    <row r="4404">
+      <c r="A4404" t="s" s="4">
+        <v>4403</v>
+      </c>
+    </row>
+    <row r="4405">
+      <c r="A4405" t="s" s="4">
+        <v>4404</v>
+      </c>
+    </row>
+    <row r="4406">
+      <c r="A4406" t="s" s="4">
+        <v>4405</v>
+      </c>
+    </row>
+    <row r="4407">
+      <c r="A4407" t="s" s="4">
+        <v>4406</v>
+      </c>
+    </row>
+    <row r="4408">
+      <c r="A4408" t="s" s="4">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="4409">
+      <c r="A4409" t="s" s="4">
+        <v>4408</v>
+      </c>
+    </row>
+    <row r="4410">
+      <c r="A4410" t="s" s="4">
+        <v>4409</v>
+      </c>
+    </row>
+    <row r="4411">
+      <c r="A4411" t="s" s="4">
+        <v>4410</v>
+      </c>
+    </row>
+    <row r="4412">
+      <c r="A4412" t="s" s="4">
+        <v>4411</v>
+      </c>
+    </row>
+    <row r="4413">
+      <c r="A4413" t="s" s="4">
+        <v>4412</v>
+      </c>
+    </row>
+    <row r="4414">
+      <c r="A4414" t="s" s="4">
+        <v>4413</v>
+      </c>
+    </row>
+    <row r="4415">
+      <c r="A4415" t="s" s="4">
+        <v>4414</v>
+      </c>
+    </row>
+    <row r="4416">
+      <c r="A4416" t="s" s="4">
+        <v>4415</v>
+      </c>
+    </row>
+    <row r="4417">
+      <c r="A4417" t="s" s="4">
+        <v>4416</v>
+      </c>
+    </row>
+    <row r="4418">
+      <c r="A4418" t="s" s="4">
+        <v>4417</v>
+      </c>
+    </row>
+    <row r="4419">
+      <c r="A4419" t="s" s="4">
+        <v>4418</v>
+      </c>
+    </row>
+    <row r="4420">
+      <c r="A4420" t="s" s="4">
+        <v>4419</v>
+      </c>
+    </row>
+    <row r="4421">
+      <c r="A4421" t="s" s="4">
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="4422">
+      <c r="A4422" t="s" s="4">
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="4423">
+      <c r="A4423" t="s" s="4">
+        <v>4422</v>
+      </c>
+    </row>
+    <row r="4424">
+      <c r="A4424" t="s" s="4">
+        <v>4423</v>
+      </c>
+    </row>
+    <row r="4425">
+      <c r="A4425" t="s" s="4">
+        <v>4424</v>
+      </c>
+    </row>
+    <row r="4426">
+      <c r="A4426" t="s" s="4">
+        <v>4425</v>
+      </c>
+    </row>
+    <row r="4427">
+      <c r="A4427" t="s" s="4">
+        <v>4426</v>
+      </c>
+    </row>
+    <row r="4428">
+      <c r="A4428" t="s" s="4">
+        <v>4427</v>
+      </c>
+    </row>
+    <row r="4429">
+      <c r="A4429" t="s" s="4">
+        <v>4428</v>
+      </c>
+    </row>
+    <row r="4430">
+      <c r="A4430" t="s" s="4">
+        <v>4429</v>
+      </c>
+    </row>
+    <row r="4431">
+      <c r="A4431" t="s" s="4">
+        <v>4430</v>
+      </c>
+    </row>
+    <row r="4432">
+      <c r="A4432" t="s" s="4">
+        <v>4431</v>
+      </c>
+    </row>
+    <row r="4433">
+      <c r="A4433" t="s" s="4">
+        <v>4432</v>
+      </c>
+    </row>
+    <row r="4434">
+      <c r="A4434" t="s" s="4">
+        <v>4433</v>
+      </c>
+    </row>
+    <row r="4435">
+      <c r="A4435" t="s" s="4">
+        <v>4434</v>
+      </c>
+    </row>
+    <row r="4436">
+      <c r="A4436" t="s" s="4">
+        <v>4435</v>
+      </c>
+    </row>
+    <row r="4437">
+      <c r="A4437" t="s" s="4">
+        <v>4436</v>
+      </c>
+    </row>
+    <row r="4438">
+      <c r="A4438" t="s" s="4">
+        <v>4437</v>
+      </c>
+    </row>
+    <row r="4439">
+      <c r="A4439" t="s" s="4">
+        <v>4438</v>
+      </c>
+    </row>
+    <row r="4440">
+      <c r="A4440" t="s" s="4">
+        <v>4439</v>
+      </c>
+    </row>
+    <row r="4441">
+      <c r="A4441" t="s" s="4">
+        <v>4440</v>
+      </c>
+    </row>
+    <row r="4442">
+      <c r="A4442" t="s" s="4">
+        <v>4441</v>
+      </c>
+    </row>
+    <row r="4443">
+      <c r="A4443" t="s" s="4">
+        <v>4442</v>
+      </c>
+    </row>
+    <row r="4444">
+      <c r="A4444" t="s" s="4">
+        <v>4443</v>
+      </c>
+    </row>
+    <row r="4445">
+      <c r="A4445" t="s" s="4">
+        <v>4444</v>
+      </c>
+    </row>
+    <row r="4446">
+      <c r="A4446" t="s" s="4">
+        <v>4445</v>
+      </c>
+    </row>
+    <row r="4447">
+      <c r="A4447" t="s" s="4">
+        <v>4446</v>
+      </c>
+    </row>
+    <row r="4448">
+      <c r="A4448" t="s" s="4">
+        <v>4447</v>
+      </c>
+    </row>
+    <row r="4449">
+      <c r="A4449" t="s" s="4">
+        <v>4448</v>
+      </c>
+    </row>
+    <row r="4450">
+      <c r="A4450" t="s" s="4">
+        <v>4449</v>
+      </c>
+    </row>
+    <row r="4451">
+      <c r="A4451" t="s" s="4">
+        <v>4450</v>
+      </c>
+    </row>
+    <row r="4452">
+      <c r="A4452" t="s" s="4">
+        <v>4451</v>
+      </c>
+    </row>
+    <row r="4453">
+      <c r="A4453" t="s" s="4">
+        <v>4452</v>
+      </c>
+    </row>
+    <row r="4454">
+      <c r="A4454" t="s" s="4">
+        <v>4453</v>
+      </c>
+    </row>
+    <row r="4455">
+      <c r="A4455" t="s" s="4">
+        <v>4454</v>
+      </c>
+    </row>
+    <row r="4456">
+      <c r="A4456" t="s" s="4">
+        <v>4455</v>
+      </c>
+    </row>
+    <row r="4457">
+      <c r="A4457" t="s" s="4">
+        <v>4456</v>
+      </c>
+    </row>
+    <row r="4458">
+      <c r="A4458" t="s" s="4">
+        <v>4457</v>
+      </c>
+    </row>
+    <row r="4459">
+      <c r="A4459" t="s" s="4">
+        <v>4458</v>
+      </c>
+    </row>
+    <row r="4460">
+      <c r="A4460" t="s" s="4">
+        <v>4459</v>
+      </c>
+    </row>
+    <row r="4461">
+      <c r="A4461" t="s" s="4">
+        <v>4460</v>
+      </c>
+    </row>
+    <row r="4462">
+      <c r="A4462" t="s" s="4">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="4463">
+      <c r="A4463" t="s" s="4">
+        <v>4462</v>
+      </c>
+    </row>
+    <row r="4464">
+      <c r="A4464" t="s" s="4">
+        <v>4463</v>
+      </c>
+    </row>
+    <row r="4465">
+      <c r="A4465" t="s" s="4">
+        <v>4464</v>
+      </c>
+    </row>
+    <row r="4466">
+      <c r="A4466" t="s" s="4">
+        <v>4465</v>
+      </c>
+    </row>
+    <row r="4467">
+      <c r="A4467" t="s" s="4">
+        <v>4466</v>
+      </c>
+    </row>
+    <row r="4468">
+      <c r="A4468" t="s" s="4">
+        <v>4467</v>
+      </c>
+    </row>
+    <row r="4469">
+      <c r="A4469" t="s" s="4">
+        <v>4468</v>
+      </c>
+    </row>
+    <row r="4470">
+      <c r="A4470" t="s" s="4">
+        <v>4469</v>
+      </c>
+    </row>
+    <row r="4471">
+      <c r="A4471" t="s" s="4">
+        <v>4470</v>
+      </c>
+    </row>
+    <row r="4472">
+      <c r="A4472" t="s" s="4">
+        <v>4471</v>
+      </c>
+    </row>
+    <row r="4473">
+      <c r="A4473" t="s" s="4">
+        <v>4472</v>
+      </c>
+    </row>
+    <row r="4474">
+      <c r="A4474" t="s" s="4">
+        <v>4473</v>
+      </c>
+    </row>
+    <row r="4475">
+      <c r="A4475" t="s" s="4">
+        <v>4474</v>
+      </c>
+    </row>
+    <row r="4476">
+      <c r="A4476" t="s" s="4">
+        <v>4475</v>
+      </c>
+    </row>
+    <row r="4477">
+      <c r="A4477" t="s" s="4">
+        <v>4476</v>
+      </c>
+    </row>
+    <row r="4478">
+      <c r="A4478" t="s" s="4">
+        <v>4477</v>
+      </c>
+    </row>
+    <row r="4479">
+      <c r="A4479" t="s" s="4">
+        <v>4478</v>
+      </c>
+    </row>
+    <row r="4480">
+      <c r="A4480" t="s" s="4">
+        <v>4479</v>
+      </c>
+    </row>
+    <row r="4481">
+      <c r="A4481" t="s" s="4">
+        <v>4480</v>
+      </c>
+    </row>
+    <row r="4482">
+      <c r="A4482" t="s" s="4">
+        <v>4481</v>
+      </c>
+    </row>
+    <row r="4483">
+      <c r="A4483" t="s" s="4">
+        <v>4482</v>
+      </c>
+    </row>
+    <row r="4484">
+      <c r="A4484" t="s" s="4">
+        <v>4483</v>
+      </c>
+    </row>
+    <row r="4485">
+      <c r="A4485" t="s" s="4">
+        <v>4484</v>
+      </c>
+    </row>
+    <row r="4486">
+      <c r="A4486" t="s" s="4">
+        <v>4485</v>
+      </c>
+    </row>
+    <row r="4487">
+      <c r="A4487" t="s" s="4">
+        <v>4486</v>
+      </c>
+    </row>
+    <row r="4488">
+      <c r="A4488" t="s" s="4">
+        <v>4487</v>
+      </c>
+    </row>
+    <row r="4489">
+      <c r="A4489" t="s" s="4">
+        <v>4488</v>
+      </c>
+    </row>
+    <row r="4490">
+      <c r="A4490" t="s" s="4">
+        <v>4489</v>
+      </c>
+    </row>
+    <row r="4491">
+      <c r="A4491" t="s" s="4">
+        <v>4490</v>
+      </c>
+    </row>
+    <row r="4492">
+      <c r="A4492" t="s" s="4">
+        <v>4491</v>
+      </c>
+    </row>
+    <row r="4493">
+      <c r="A4493" t="s" s="4">
+        <v>4492</v>
+      </c>
+    </row>
+    <row r="4494">
+      <c r="A4494" t="s" s="4">
+        <v>4493</v>
+      </c>
+    </row>
+    <row r="4495">
+      <c r="A4495" t="s" s="4">
+        <v>4494</v>
+      </c>
+    </row>
+    <row r="4496">
+      <c r="A4496" t="s" s="4">
+        <v>4495</v>
+      </c>
+    </row>
+    <row r="4497">
+      <c r="A4497" t="s" s="4">
+        <v>4496</v>
+      </c>
+    </row>
+    <row r="4498">
+      <c r="A4498" t="s" s="4">
+        <v>4497</v>
+      </c>
+    </row>
+    <row r="4499">
+      <c r="A4499" t="s" s="4">
+        <v>4498</v>
+      </c>
+    </row>
+    <row r="4500">
+      <c r="A4500" t="s" s="4">
+        <v>4499</v>
+      </c>
+    </row>
+    <row r="4501">
+      <c r="A4501" t="s" s="4">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="4502">
+      <c r="A4502" t="s" s="4">
+        <v>4501</v>
+      </c>
+    </row>
+    <row r="4503">
+      <c r="A4503" t="s" s="4">
+        <v>4502</v>
+      </c>
+    </row>
+    <row r="4504">
+      <c r="A4504" t="s" s="4">
+        <v>4503</v>
+      </c>
+    </row>
+    <row r="4505">
+      <c r="A4505" t="s" s="4">
+        <v>4504</v>
+      </c>
+    </row>
+    <row r="4506">
+      <c r="A4506" t="s" s="4">
+        <v>4505</v>
+      </c>
+    </row>
+    <row r="4507">
+      <c r="A4507" t="s" s="4">
+        <v>4506</v>
+      </c>
+    </row>
+    <row r="4508">
+      <c r="A4508" t="s" s="4">
+        <v>4507</v>
+      </c>
+    </row>
+    <row r="4509">
+      <c r="A4509" t="s" s="4">
+        <v>4508</v>
+      </c>
+    </row>
+    <row r="4510">
+      <c r="A4510" t="s" s="4">
+        <v>4509</v>
+      </c>
+    </row>
+    <row r="4511">
+      <c r="A4511" t="s" s="4">
+        <v>4510</v>
+      </c>
+    </row>
+    <row r="4512">
+      <c r="A4512" t="s" s="4">
+        <v>4511</v>
+      </c>
+    </row>
+    <row r="4513">
+      <c r="A4513" t="s" s="4">
+        <v>4512</v>
+      </c>
+    </row>
+    <row r="4514">
+      <c r="A4514" t="s" s="4">
+        <v>4513</v>
+      </c>
+    </row>
+    <row r="4515">
+      <c r="A4515" t="s" s="4">
+        <v>4514</v>
+      </c>
+    </row>
+    <row r="4516">
+      <c r="A4516" t="s" s="4">
+        <v>4515</v>
+      </c>
+    </row>
+    <row r="4517">
+      <c r="A4517" t="s" s="4">
+        <v>4516</v>
+      </c>
+    </row>
+    <row r="4518">
+      <c r="A4518" t="s" s="4">
+        <v>4517</v>
+      </c>
+    </row>
+    <row r="4519">
+      <c r="A4519" t="s" s="4">
+        <v>4518</v>
+      </c>
+    </row>
+    <row r="4520">
+      <c r="A4520" t="s" s="4">
+        <v>4519</v>
+      </c>
+    </row>
+    <row r="4521">
+      <c r="A4521" t="s" s="4">
+        <v>4520</v>
+      </c>
+    </row>
+    <row r="4522">
+      <c r="A4522" t="s" s="4">
+        <v>4521</v>
+      </c>
+    </row>
+    <row r="4523">
+      <c r="A4523" t="s" s="4">
+        <v>4522</v>
+      </c>
+    </row>
+    <row r="4524">
+      <c r="A4524" t="s" s="4">
+        <v>4523</v>
+      </c>
+    </row>
+    <row r="4525">
+      <c r="A4525" t="s" s="4">
+        <v>4524</v>
+      </c>
+    </row>
+    <row r="4526">
+      <c r="A4526" t="s" s="4">
+        <v>4525</v>
+      </c>
+    </row>
+    <row r="4527">
+      <c r="A4527" t="s" s="4">
+        <v>4526</v>
+      </c>
+    </row>
+    <row r="4528">
+      <c r="A4528" t="s" s="4">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4529">
+      <c r="A4529" t="s" s="4">
+        <v>4528</v>
+      </c>
+    </row>
+    <row r="4530">
+      <c r="A4530" t="s" s="4">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4531">
+      <c r="A4531" t="s" s="4">
+        <v>4530</v>
+      </c>
+    </row>
+    <row r="4532">
+      <c r="A4532" t="s" s="4">
+        <v>4531</v>
+      </c>
+    </row>
+    <row r="4533">
+      <c r="A4533" t="s" s="4">
+        <v>4532</v>
+      </c>
+    </row>
+    <row r="4534">
+      <c r="A4534" t="s" s="4">
+        <v>4533</v>
+      </c>
+    </row>
+    <row r="4535">
+      <c r="A4535" t="s" s="4">
+        <v>4534</v>
+      </c>
+    </row>
+    <row r="4536">
+      <c r="A4536" t="s" s="4">
+        <v>4535</v>
+      </c>
+    </row>
+    <row r="4537">
+      <c r="A4537" t="s" s="4">
+        <v>4536</v>
+      </c>
+    </row>
+    <row r="4538">
+      <c r="A4538" t="s" s="4">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="4539">
+      <c r="A4539" t="s" s="4">
+        <v>4538</v>
+      </c>
+    </row>
+    <row r="4540">
+      <c r="A4540" t="s" s="4">
+        <v>4539</v>
+      </c>
+    </row>
+    <row r="4541">
+      <c r="A4541" t="s" s="4">
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="4542">
+      <c r="A4542" t="s" s="4">
+        <v>4541</v>
+      </c>
+    </row>
+    <row r="4543">
+      <c r="A4543" t="s" s="4">
+        <v>4542</v>
+      </c>
+    </row>
+    <row r="4544">
+      <c r="A4544" t="s" s="4">
+        <v>4543</v>
+      </c>
+    </row>
+    <row r="4545">
+      <c r="A4545" t="s" s="4">
+        <v>4544</v>
+      </c>
+    </row>
+    <row r="4546">
+      <c r="A4546" t="s" s="4">
+        <v>4545</v>
+      </c>
+    </row>
+    <row r="4547">
+      <c r="A4547" t="s" s="4">
+        <v>4546</v>
+      </c>
+    </row>
+    <row r="4548">
+      <c r="A4548" t="s" s="4">
+        <v>4547</v>
+      </c>
+    </row>
+    <row r="4549">
+      <c r="A4549" t="s" s="4">
+        <v>4548</v>
+      </c>
+    </row>
+    <row r="4550">
+      <c r="A4550" t="s" s="4">
+        <v>4549</v>
+      </c>
+    </row>
+    <row r="4551">
+      <c r="A4551" t="s" s="4">
+        <v>4550</v>
+      </c>
+    </row>
+    <row r="4552">
+      <c r="A4552" t="s" s="4">
+        <v>4551</v>
+      </c>
+    </row>
+    <row r="4553">
+      <c r="A4553" t="s" s="4">
+        <v>4552</v>
+      </c>
+    </row>
+    <row r="4554">
+      <c r="A4554" t="s" s="4">
+        <v>4553</v>
+      </c>
+    </row>
+    <row r="4555">
+      <c r="A4555" t="s" s="4">
+        <v>4554</v>
+      </c>
+    </row>
+    <row r="4556">
+      <c r="A4556" t="s" s="4">
+        <v>4555</v>
+      </c>
+    </row>
+    <row r="4557">
+      <c r="A4557" t="s" s="4">
+        <v>4556</v>
+      </c>
+    </row>
+    <row r="4558">
+      <c r="A4558" t="s" s="4">
+        <v>4557</v>
+      </c>
+    </row>
+    <row r="4559">
+      <c r="A4559" t="s" s="4">
+        <v>4558</v>
+      </c>
+    </row>
+    <row r="4560">
+      <c r="A4560" t="s" s="4">
+        <v>4559</v>
+      </c>
+    </row>
+    <row r="4561">
+      <c r="A4561" t="s" s="4">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="4562">
+      <c r="A4562" t="s" s="4">
+        <v>4561</v>
+      </c>
+    </row>
+    <row r="4563">
+      <c r="A4563" t="s" s="4">
+        <v>4562</v>
+      </c>
+    </row>
+    <row r="4564">
+      <c r="A4564" t="s" s="4">
+        <v>4563</v>
+      </c>
+    </row>
+    <row r="4565">
+      <c r="A4565" t="s" s="4">
+        <v>4564</v>
+      </c>
+    </row>
+    <row r="4566">
+      <c r="A4566" t="s" s="4">
+        <v>4565</v>
+      </c>
+    </row>
+    <row r="4567">
+      <c r="A4567" t="s" s="4">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="4568">
+      <c r="A4568" t="s" s="4">
+        <v>4567</v>
+      </c>
+    </row>
+    <row r="4569">
+      <c r="A4569" t="s" s="4">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="4570">
+      <c r="A4570" t="s" s="4">
+        <v>4569</v>
+      </c>
+    </row>
+    <row r="4571">
+      <c r="A4571" t="s" s="4">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="4572">
+      <c r="A4572" t="s" s="4">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="4573">
+      <c r="A4573" t="s" s="4">
+        <v>4572</v>
+      </c>
+    </row>
+    <row r="4574">
+      <c r="A4574" t="s" s="4">
+        <v>4573</v>
+      </c>
+    </row>
+    <row r="4575">
+      <c r="A4575" t="s" s="4">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="4576">
+      <c r="A4576" t="s" s="4">
+        <v>4575</v>
+      </c>
+    </row>
+    <row r="4577">
+      <c r="A4577" t="s" s="4">
+        <v>4576</v>
+      </c>
+    </row>
+    <row r="4578">
+      <c r="A4578" t="s" s="4">
+        <v>4577</v>
+      </c>
+    </row>
+    <row r="4579">
+      <c r="A4579" t="s" s="4">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="4580">
+      <c r="A4580" t="s" s="4">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="4581">
+      <c r="A4581" t="s" s="4">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="4582">
+      <c r="A4582" t="s" s="4">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="4583">
+      <c r="A4583" t="s" s="4">
+        <v>4582</v>
+      </c>
+    </row>
+    <row r="4584">
+      <c r="A4584" t="s" s="4">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="4585">
+      <c r="A4585" t="s" s="4">
+        <v>4584</v>
+      </c>
+    </row>
+    <row r="4586">
+      <c r="A4586" t="s" s="4">
+        <v>4585</v>
+      </c>
+    </row>
+    <row r="4587">
+      <c r="A4587" t="s" s="4">
+        <v>4586</v>
+      </c>
+    </row>
+    <row r="4588">
+      <c r="A4588" t="s" s="4">
+        <v>4587</v>
+      </c>
+    </row>
+    <row r="4589">
+      <c r="A4589" t="s" s="4">
+        <v>4588</v>
+      </c>
+    </row>
+    <row r="4590">
+      <c r="A4590" t="s" s="4">
+        <v>4589</v>
+      </c>
+    </row>
+    <row r="4591">
+      <c r="A4591" t="s" s="4">
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="4592">
+      <c r="A4592" t="s" s="4">
+        <v>4591</v>
+      </c>
+    </row>
+    <row r="4593">
+      <c r="A4593" t="s" s="4">
+        <v>4592</v>
+      </c>
+    </row>
+    <row r="4594">
+      <c r="A4594" t="s" s="4">
+        <v>4593</v>
+      </c>
+    </row>
+    <row r="4595">
+      <c r="A4595" t="s" s="4">
+        <v>4594</v>
+      </c>
+    </row>
+    <row r="4596">
+      <c r="A4596" t="s" s="4">
+        <v>4595</v>
+      </c>
+    </row>
+    <row r="4597">
+      <c r="A4597" t="s" s="4">
+        <v>4596</v>
+      </c>
+    </row>
+    <row r="4598">
+      <c r="A4598" t="s" s="4">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="4599">
+      <c r="A4599" t="s" s="4">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="4600">
+      <c r="A4600" t="s" s="4">
+        <v>4599</v>
+      </c>
+    </row>
+    <row r="4601">
+      <c r="A4601" t="s" s="4">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="4602">
+      <c r="A4602" t="s" s="4">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="4603">
+      <c r="A4603" t="s" s="4">
+        <v>4602</v>
+      </c>
+    </row>
+    <row r="4604">
+      <c r="A4604" t="s" s="4">
+        <v>4603</v>
+      </c>
+    </row>
+    <row r="4605">
+      <c r="A4605" t="s" s="4">
+        <v>4604</v>
+      </c>
+    </row>
+    <row r="4606">
+      <c r="A4606" t="s" s="4">
+        <v>4605</v>
+      </c>
+    </row>
+    <row r="4607">
+      <c r="A4607" t="s" s="4">
+        <v>4606</v>
+      </c>
+    </row>
+    <row r="4608">
+      <c r="A4608" t="s" s="4">
+        <v>4607</v>
+      </c>
+    </row>
+    <row r="4609">
+      <c r="A4609" t="s" s="4">
+        <v>4608</v>
+      </c>
+    </row>
+    <row r="4610">
+      <c r="A4610" t="s" s="4">
+        <v>4609</v>
+      </c>
+    </row>
+    <row r="4611">
+      <c r="A4611" t="s" s="4">
+        <v>4610</v>
+      </c>
+    </row>
+    <row r="4612">
+      <c r="A4612" t="s" s="4">
+        <v>4611</v>
+      </c>
+    </row>
+    <row r="4613">
+      <c r="A4613" t="s" s="4">
+        <v>4612</v>
+      </c>
+    </row>
+    <row r="4614">
+      <c r="A4614" t="s" s="4">
+        <v>4613</v>
+      </c>
+    </row>
+    <row r="4615">
+      <c r="A4615" t="s" s="4">
+        <v>4614</v>
+      </c>
+    </row>
+    <row r="4616">
+      <c r="A4616" t="s" s="4">
+        <v>4615</v>
+      </c>
+    </row>
+    <row r="4617">
+      <c r="A4617" t="s" s="4">
+        <v>4616</v>
+      </c>
+    </row>
+    <row r="4618">
+      <c r="A4618" t="s" s="4">
+        <v>4617</v>
+      </c>
+    </row>
+    <row r="4619">
+      <c r="A4619" t="s" s="4">
+        <v>4618</v>
+      </c>
+    </row>
+    <row r="4620">
+      <c r="A4620" t="s" s="4">
+        <v>4619</v>
+      </c>
+    </row>
+    <row r="4621">
+      <c r="A4621" t="s" s="4">
+        <v>4620</v>
+      </c>
+    </row>
+    <row r="4622">
+      <c r="A4622" t="s" s="4">
+        <v>4621</v>
+      </c>
+    </row>
+    <row r="4623">
+      <c r="A4623" t="s" s="4">
+        <v>4622</v>
+      </c>
+    </row>
+    <row r="4624">
+      <c r="A4624" t="s" s="4">
+        <v>4623</v>
+      </c>
+    </row>
+    <row r="4625">
+      <c r="A4625" t="s" s="4">
+        <v>4624</v>
+      </c>
+    </row>
+    <row r="4626">
+      <c r="A4626" t="s" s="4">
+        <v>4625</v>
+      </c>
+    </row>
+    <row r="4627">
+      <c r="A4627" t="s" s="4">
+        <v>4626</v>
+      </c>
+    </row>
+    <row r="4628">
+      <c r="A4628" t="s" s="4">
+        <v>4627</v>
+      </c>
+    </row>
+    <row r="4629">
+      <c r="A4629" t="s" s="4">
+        <v>4628</v>
+      </c>
+    </row>
+    <row r="4630">
+      <c r="A4630" t="s" s="4">
+        <v>4629</v>
+      </c>
+    </row>
+    <row r="4631">
+      <c r="A4631" t="s" s="4">
+        <v>4630</v>
+      </c>
+    </row>
+    <row r="4632">
+      <c r="A4632" t="s" s="4">
+        <v>4631</v>
+      </c>
+    </row>
+    <row r="4633">
+      <c r="A4633" t="s" s="4">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="4634">
+      <c r="A4634" t="s" s="4">
+        <v>4633</v>
+      </c>
+    </row>
+    <row r="4635">
+      <c r="A4635" t="s" s="4">
+        <v>4634</v>
+      </c>
+    </row>
+    <row r="4636">
+      <c r="A4636" t="s" s="4">
+        <v>4635</v>
+      </c>
+    </row>
+    <row r="4637">
+      <c r="A4637" t="s" s="4">
+        <v>4636</v>
+      </c>
+    </row>
+    <row r="4638">
+      <c r="A4638" t="s" s="4">
+        <v>4637</v>
+      </c>
+    </row>
+    <row r="4639">
+      <c r="A4639" t="s" s="4">
+        <v>4638</v>
+      </c>
+    </row>
+    <row r="4640">
+      <c r="A4640" t="s" s="4">
+        <v>4639</v>
+      </c>
+    </row>
+    <row r="4641">
+      <c r="A4641" t="s" s="4">
+        <v>4640</v>
+      </c>
+    </row>
+    <row r="4642">
+      <c r="A4642" t="s" s="4">
+        <v>4641</v>
+      </c>
+    </row>
+    <row r="4643">
+      <c r="A4643" t="s" s="4">
+        <v>4642</v>
+      </c>
+    </row>
+    <row r="4644">
+      <c r="A4644" t="s" s="4">
+        <v>4643</v>
+      </c>
+    </row>
+    <row r="4645">
+      <c r="A4645" t="s" s="4">
+        <v>4644</v>
+      </c>
+    </row>
+    <row r="4646">
+      <c r="A4646" t="s" s="4">
+        <v>4645</v>
+      </c>
+    </row>
+    <row r="4647">
+      <c r="A4647" t="s" s="4">
+        <v>4646</v>
+      </c>
+    </row>
+    <row r="4648">
+      <c r="A4648" t="s" s="4">
+        <v>4647</v>
+      </c>
+    </row>
+    <row r="4649">
+      <c r="A4649" t="s" s="4">
+        <v>4648</v>
+      </c>
+    </row>
+    <row r="4650">
+      <c r="A4650" t="s" s="4">
+        <v>4649</v>
+      </c>
+    </row>
+    <row r="4651">
+      <c r="A4651" t="s" s="4">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="4652">
+      <c r="A4652" t="s" s="4">
+        <v>4651</v>
+      </c>
+    </row>
+    <row r="4653">
+      <c r="A4653" t="s" s="4">
+        <v>4652</v>
+      </c>
+    </row>
+    <row r="4654">
+      <c r="A4654" t="s" s="4">
+        <v>4653</v>
+      </c>
+    </row>
+    <row r="4655">
+      <c r="A4655" t="s" s="4">
+        <v>4654</v>
+      </c>
+    </row>
+    <row r="4656">
+      <c r="A4656" t="s" s="4">
+        <v>4655</v>
+      </c>
+    </row>
+    <row r="4657">
+      <c r="A4657" t="s" s="4">
+        <v>4656</v>
+      </c>
+    </row>
+    <row r="4658">
+      <c r="A4658" t="s" s="4">
+        <v>4657</v>
+      </c>
+    </row>
+    <row r="4659">
+      <c r="A4659" t="s" s="4">
+        <v>4658</v>
+      </c>
+    </row>
+    <row r="4660">
+      <c r="A4660" t="s" s="4">
+        <v>4659</v>
+      </c>
+    </row>
+    <row r="4661">
+      <c r="A4661" t="s" s="4">
+        <v>4660</v>
+      </c>
+    </row>
+    <row r="4662">
+      <c r="A4662" t="s" s="4">
+        <v>4661</v>
+      </c>
+    </row>
+    <row r="4663">
+      <c r="A4663" t="s" s="4">
+        <v>4662</v>
+      </c>
+    </row>
+    <row r="4664">
+      <c r="A4664" t="s" s="4">
+        <v>4663</v>
+      </c>
+    </row>
+    <row r="4665">
+      <c r="A4665" t="s" s="4">
+        <v>4664</v>
+      </c>
+    </row>
+    <row r="4666">
+      <c r="A4666" t="s" s="4">
+        <v>4665</v>
+      </c>
+    </row>
+    <row r="4667">
+      <c r="A4667" t="s" s="4">
+        <v>4666</v>
+      </c>
+    </row>
+    <row r="4668">
+      <c r="A4668" t="s" s="4">
+        <v>4667</v>
+      </c>
+    </row>
+    <row r="4669">
+      <c r="A4669" t="s" s="4">
+        <v>4668</v>
+      </c>
+    </row>
+    <row r="4670">
+      <c r="A4670" t="s" s="4">
+        <v>4669</v>
+      </c>
+    </row>
+    <row r="4671">
+      <c r="A4671" t="s" s="4">
+        <v>4670</v>
+      </c>
+    </row>
+    <row r="4672">
+      <c r="A4672" t="s" s="4">
+        <v>4671</v>
+      </c>
+    </row>
+    <row r="4673">
+      <c r="A4673" t="s" s="4">
+        <v>4672</v>
+      </c>
+    </row>
+    <row r="4674">
+      <c r="A4674" t="s" s="4">
+        <v>4673</v>
+      </c>
+    </row>
+    <row r="4675">
+      <c r="A4675" t="s" s="4">
+        <v>4674</v>
+      </c>
+    </row>
+    <row r="4676">
+      <c r="A4676" t="s" s="4">
+        <v>4675</v>
+      </c>
+    </row>
+    <row r="4677">
+      <c r="A4677" t="s" s="4">
+        <v>4676</v>
+      </c>
+    </row>
+    <row r="4678">
+      <c r="A4678" t="s" s="4">
+        <v>4677</v>
+      </c>
+    </row>
+    <row r="4679">
+      <c r="A4679" t="s" s="4">
+        <v>4678</v>
+      </c>
+    </row>
+    <row r="4680">
+      <c r="A4680" t="s" s="4">
+        <v>4679</v>
+      </c>
+    </row>
+    <row r="4681">
+      <c r="A4681" t="s" s="4">
+        <v>4680</v>
+      </c>
+    </row>
+    <row r="4682">
+      <c r="A4682" t="s" s="4">
+        <v>4681</v>
+      </c>
+    </row>
+    <row r="4683">
+      <c r="A4683" t="s" s="4">
+        <v>4682</v>
+      </c>
+    </row>
+    <row r="4684">
+      <c r="A4684" t="s" s="4">
+        <v>4683</v>
+      </c>
+    </row>
+    <row r="4685">
+      <c r="A4685" t="s" s="4">
+        <v>4684</v>
+      </c>
+    </row>
+    <row r="4686">
+      <c r="A4686" t="s" s="4">
+        <v>4685</v>
+      </c>
+    </row>
+    <row r="4687">
+      <c r="A4687" t="s" s="4">
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="4688">
+      <c r="A4688" t="s" s="4">
+        <v>4687</v>
+      </c>
+    </row>
+    <row r="4689">
+      <c r="A4689" t="s" s="4">
+        <v>4688</v>
+      </c>
+    </row>
+    <row r="4690">
+      <c r="A4690" t="s" s="4">
+        <v>4689</v>
+      </c>
+    </row>
+    <row r="4691">
+      <c r="A4691" t="s" s="4">
+        <v>4690</v>
+      </c>
+    </row>
+    <row r="4692">
+      <c r="A4692" t="s" s="4">
+        <v>4691</v>
+      </c>
+    </row>
+    <row r="4693">
+      <c r="A4693" t="s" s="4">
+        <v>4692</v>
+      </c>
+    </row>
+    <row r="4694">
+      <c r="A4694" t="s" s="4">
+        <v>4693</v>
+      </c>
+    </row>
+    <row r="4695">
+      <c r="A4695" t="s" s="4">
+        <v>4694</v>
+      </c>
+    </row>
+    <row r="4696">
+      <c r="A4696" t="s" s="4">
+        <v>4695</v>
+      </c>
+    </row>
+    <row r="4697">
+      <c r="A4697" t="s" s="4">
+        <v>4696</v>
+      </c>
+    </row>
+    <row r="4698">
+      <c r="A4698" t="s" s="4">
+        <v>4697</v>
+      </c>
+    </row>
+    <row r="4699">
+      <c r="A4699" t="s" s="4">
+        <v>4698</v>
+      </c>
+    </row>
+    <row r="4700">
+      <c r="A4700" t="s" s="4">
+        <v>4699</v>
+      </c>
+    </row>
+    <row r="4701">
+      <c r="A4701" t="s" s="4">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="4702">
+      <c r="A4702" t="s" s="4">
+        <v>4701</v>
+      </c>
+    </row>
+    <row r="4703">
+      <c r="A4703" t="s" s="4">
+        <v>4702</v>
+      </c>
+    </row>
+    <row r="4704">
+      <c r="A4704" t="s" s="4">
+        <v>4703</v>
+      </c>
+    </row>
+    <row r="4705">
+      <c r="A4705" t="s" s="4">
+        <v>4704</v>
+      </c>
+    </row>
+    <row r="4706">
+      <c r="A4706" t="s" s="4">
+        <v>4705</v>
+      </c>
+    </row>
+    <row r="4707">
+      <c r="A4707" t="s" s="4">
+        <v>4706</v>
+      </c>
+    </row>
+    <row r="4708">
+      <c r="A4708" t="s" s="4">
+        <v>4707</v>
+      </c>
+    </row>
+    <row r="4709">
+      <c r="A4709" t="s" s="4">
+        <v>4708</v>
+      </c>
+    </row>
+    <row r="4710">
+      <c r="A4710" t="s" s="4">
+        <v>4709</v>
+      </c>
+    </row>
+    <row r="4711">
+      <c r="A4711" t="s" s="4">
+        <v>4710</v>
+      </c>
+    </row>
+    <row r="4712">
+      <c r="A4712" t="s" s="4">
+        <v>4711</v>
+      </c>
+    </row>
+    <row r="4713">
+      <c r="A4713" t="s" s="4">
+        <v>4712</v>
+      </c>
+    </row>
+    <row r="4714">
+      <c r="A4714" t="s" s="4">
+        <v>4713</v>
+      </c>
+    </row>
+    <row r="4715">
+      <c r="A4715" t="s" s="4">
+        <v>4714</v>
+      </c>
+    </row>
+    <row r="4716">
+      <c r="A4716" t="s" s="4">
+        <v>4715</v>
+      </c>
+    </row>
+    <row r="4717">
+      <c r="A4717" t="s" s="4">
+        <v>4716</v>
+      </c>
+    </row>
+    <row r="4718">
+      <c r="A4718" t="s" s="4">
+        <v>4717</v>
+      </c>
+    </row>
+    <row r="4719">
+      <c r="A4719" t="s" s="4">
+        <v>4718</v>
+      </c>
+    </row>
+    <row r="4720">
+      <c r="A4720" t="s" s="4">
+        <v>4719</v>
+      </c>
+    </row>
+    <row r="4721">
+      <c r="A4721" t="s" s="4">
+        <v>4720</v>
+      </c>
+    </row>
+    <row r="4722">
+      <c r="A4722" t="s" s="4">
+        <v>4721</v>
+      </c>
+    </row>
+    <row r="4723">
+      <c r="A4723" t="s" s="4">
+        <v>4722</v>
+      </c>
+    </row>
+    <row r="4724">
+      <c r="A4724" t="s" s="4">
+        <v>4723</v>
+      </c>
+    </row>
+    <row r="4725">
+      <c r="A4725" t="s" s="4">
+        <v>4724</v>
+      </c>
+    </row>
+    <row r="4726">
+      <c r="A4726" t="s" s="4">
+        <v>4725</v>
+      </c>
+    </row>
+    <row r="4727">
+      <c r="A4727" t="s" s="4">
+        <v>4726</v>
+      </c>
+    </row>
+    <row r="4728">
+      <c r="A4728" t="s" s="4">
+        <v>4727</v>
+      </c>
+    </row>
+    <row r="4729">
+      <c r="A4729" t="s" s="4">
+        <v>4728</v>
+      </c>
+    </row>
+    <row r="4730">
+      <c r="A4730" t="s" s="4">
+        <v>4729</v>
+      </c>
+    </row>
+    <row r="4731">
+      <c r="A4731" t="s" s="4">
+        <v>4730</v>
+      </c>
+    </row>
+    <row r="4732">
+      <c r="A4732" t="s" s="4">
+        <v>4731</v>
+      </c>
+    </row>
+    <row r="4733">
+      <c r="A4733" t="s" s="4">
+        <v>4732</v>
+      </c>
+    </row>
+    <row r="4734">
+      <c r="A4734" t="s" s="4">
+        <v>4733</v>
+      </c>
+    </row>
+    <row r="4735">
+      <c r="A4735" t="s" s="4">
+        <v>4734</v>
+      </c>
+    </row>
+    <row r="4736">
+      <c r="A4736" t="s" s="4">
+        <v>4735</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>